<commit_message>
filelist 추가 nav 변경 admin 추가
</commit_message>
<xml_diff>
--- a/#file/List_FileName.xlsx
+++ b/#file/List_FileName.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>header.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -286,6 +286,26 @@
   </si>
   <si>
     <t>추가삽입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>momoaInsertData.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin_input.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템 정보 삽입 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin work sheet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템 정보 디비 삽입($conn)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -335,7 +355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,6 +368,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -737,7 +763,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -953,6 +979,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,10 +1307,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H31"/>
+  <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1662,8 +1721,51 @@
         <v>62</v>
       </c>
     </row>
+    <row r="35" spans="2:8" ht="3.95" customHeight="1"/>
+    <row r="36" spans="2:8" ht="29.25" customHeight="1">
+      <c r="B36" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="72"/>
+    </row>
+    <row r="37" spans="2:8" ht="3.95" customHeight="1" thickBot="1"/>
+    <row r="38" spans="2:8">
+      <c r="B38" s="73">
+        <v>17</v>
+      </c>
+      <c r="C38" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="77" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="17.25" thickBot="1">
+      <c r="B39" s="78">
+        <v>18</v>
+      </c>
+      <c r="C39" s="79" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="79"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="80"/>
+      <c r="G39" s="81" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" s="82" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B25:C25"/>

</xml_diff>